<commit_message>
Syncing master branch with beta
</commit_message>
<xml_diff>
--- a/Background Documentation/Burndown Chart/Burndown_Chart.xlsx
+++ b/Background Documentation/Burndown Chart/Burndown_Chart.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maddy Carden\Documents\UNI\Semester 1 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maddy Carden\Documents\UNI\Semester 2 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A34D0E-1C75-4C68-8F07-D656E69F4CEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F89C2FFE-0ABD-4645-86BB-EE34303A6ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1C7A58D7-4E6D-4B99-A39A-FCECED6FF1E1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Semester 2" sheetId="2" r:id="rId1"/>
+    <sheet name="Semester 1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>User Story</t>
   </si>
@@ -169,13 +170,64 @@
   </si>
   <si>
     <t>Start</t>
+  </si>
+  <si>
+    <t>1.1.9. As a user, I want to detect and access the ambient light sensor so that I can gather ambient light data</t>
+  </si>
+  <si>
+    <t>1.1.10. As a user, I want to detect and access the GPS so that I can gather latitude and longitude data</t>
+  </si>
+  <si>
+    <t>1.1.11. As a user, I want microphone data to be collected without lag in real time so that all my data can be collected in unison</t>
+  </si>
+  <si>
+    <t>1.2.8. As a user I want to collect illuminance from the ambient light sensor so that I have this data for my experiment</t>
+  </si>
+  <si>
+    <t>1.2.9. As a user I want to collect latitude and longitude from the GPS so that I have this data for my experiment</t>
+  </si>
+  <si>
+    <t>2.2.7. As a user I want to generate and update a graph for ambient light luminosity data in real-time, so that I can view my collected data</t>
+  </si>
+  <si>
+    <t>2.2.8. As a user I want to generate and update a graph for GPS latitude and longitude data in real-time so that I can view my collected data</t>
+  </si>
+  <si>
+    <t>3.1.8. As a user I want to store the collected ambient light luminosity, so that I can use it later</t>
+  </si>
+  <si>
+    <t>3.1.9. As a user I want to store the collected GPS latitude and longitude data, so that I can use it later</t>
+  </si>
+  <si>
+    <t>3.2.4. As a user, I want to delete data that I have exported, so that my device storage doesn't fill up with data once I have finished using it</t>
+  </si>
+  <si>
+    <t>4.1.1. As a developer, I want to obtain ethical clearance so that I can test the application with disabled individuals</t>
+  </si>
+  <si>
+    <t>4.1.2. As a developer, I want to test the application with disabled users so that I can optimize the usability of the application</t>
+  </si>
+  <si>
+    <t>4.1.3. As a product owner, I want an apk, so that I can test the android app myself</t>
+  </si>
+  <si>
+    <t>4.1.4. As a product owner, I want an ipa so that I can test the iOS app myself</t>
+  </si>
+  <si>
+    <t>Sprint 9</t>
+  </si>
+  <si>
+    <t>Sprint 10</t>
+  </si>
+  <si>
+    <t>Ideal work remaining</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +248,19 @@
       <color rgb="FF1A1A1A"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,10 +283,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,6 +306,472 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Sensible Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal work remaining</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Semester 2'!$C$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sprint 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Sprint 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sprint 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sprint 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Sprint 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Semester 2'!$C$19:$M$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>163.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>145.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>127.40000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>109.20000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91.000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72.800000000000011</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F7F0-4C7D-A920-8F630EB03D2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual work remaining</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Semester 2'!$C$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sprint 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Sprint 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sprint 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sprint 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Sprint 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Semester 2'!$C$18:$M$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-F7F0-4C7D-A920-8F630EB03D2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="221237856"/>
+        <c:axId val="221238688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="221237856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="221238688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="221238688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="221237856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -324,7 +856,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$36</c:f>
+              <c:f>'Semester 1'!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -347,7 +879,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:f>'Semester 1'!$B$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -382,7 +914,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$36:$J$36</c:f>
+              <c:f>'Semester 1'!$B$36:$J$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -428,7 +960,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$37</c:f>
+              <c:f>'Semester 1'!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -451,7 +983,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:f>'Semester 1'!$B$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -486,7 +1018,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$37:$J$37</c:f>
+              <c:f>'Semester 1'!$B$37:$J$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -509,7 +1041,10 @@
                   <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>111</c:v>
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -818,6 +1353,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1334,7 +1909,564 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95557</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>26230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>311274</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>149411</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EBF2B69-DDAA-4DC8-A972-C8CAAB024B4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1671,14 +2803,339 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8D38B7-E15B-446D-AF9D-70DAFFF397FD}">
+  <dimension ref="A1:M34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="51" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="52.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <f>SUM(C2:C15)</f>
+        <v>182</v>
+      </c>
+      <c r="D18">
+        <f>C18-SUM(D5:D15)</f>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>182</v>
+      </c>
+      <c r="D19">
+        <f>C19-18.2</f>
+        <v>163.80000000000001</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:M19" si="0">D19-18.2</f>
+        <v>145.60000000000002</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>127.40000000000002</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>109.20000000000002</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>91.000000000000014</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>72.800000000000011</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>54.600000000000009</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>36.400000000000006</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>18.200000000000006</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF4A8D6-7B70-4B05-B2EF-CB4408646652}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="47" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J34"/>
+    <sheetView zoomScale="40" workbookViewId="0">
+      <selection sqref="A1:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1744,6 +3201,12 @@
       <c r="H2">
         <v>6</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1770,6 +3233,12 @@
       <c r="H3">
         <v>0</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -1796,6 +3265,12 @@
       <c r="H4">
         <v>6</v>
       </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -1822,6 +3297,12 @@
       <c r="H5">
         <v>0</v>
       </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -1848,6 +3329,12 @@
       <c r="H6">
         <v>6</v>
       </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
@@ -1874,6 +3361,12 @@
       <c r="H7">
         <v>0</v>
       </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -1900,6 +3393,12 @@
       <c r="H8">
         <v>0</v>
       </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
@@ -1924,6 +3423,12 @@
         <v>0</v>
       </c>
       <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
         <v>0</v>
       </c>
     </row>
@@ -1952,6 +3457,12 @@
       <c r="H10">
         <v>8</v>
       </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
@@ -1978,6 +3489,12 @@
       <c r="H11">
         <v>0</v>
       </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
@@ -2004,6 +3521,12 @@
       <c r="H12">
         <v>8</v>
       </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
@@ -2030,6 +3553,12 @@
       <c r="H13">
         <v>8</v>
       </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
@@ -2056,6 +3585,12 @@
       <c r="H14">
         <v>0</v>
       </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
@@ -2082,6 +3617,12 @@
       <c r="H15">
         <v>0</v>
       </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
@@ -2108,8 +3649,14 @@
       <c r="H16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -2134,8 +3681,14 @@
       <c r="H17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -2160,8 +3713,14 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -2186,8 +3745,14 @@
       <c r="H19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2212,8 +3777,14 @@
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -2238,8 +3809,14 @@
       <c r="H21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2264,8 +3841,14 @@
       <c r="H22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2290,8 +3873,14 @@
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2316,8 +3905,14 @@
       <c r="H24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2342,8 +3937,14 @@
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25">
+        <v>8</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2368,8 +3969,14 @@
       <c r="H26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -2394,8 +4001,14 @@
       <c r="H27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27">
+        <v>8</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2420,8 +4033,14 @@
       <c r="H28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -2446,8 +4065,14 @@
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29">
+        <v>8</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2472,8 +4097,14 @@
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30">
+        <v>8</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -2498,8 +4129,14 @@
       <c r="H31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -2522,6 +4159,12 @@
         <v>0</v>
       </c>
       <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>8</v>
+      </c>
+      <c r="J32">
         <v>0</v>
       </c>
     </row>
@@ -2550,6 +4193,12 @@
       <c r="H33">
         <v>0</v>
       </c>
+      <c r="I33">
+        <v>8</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
@@ -2576,6 +4225,12 @@
       <c r="H34">
         <v>0</v>
       </c>
+      <c r="I34">
+        <v>13</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
@@ -2642,12 +4297,16 @@
         <v>223</v>
       </c>
       <c r="G37">
-        <f t="shared" ref="G37:J37" si="1">F37-SUM(G2:G34)</f>
+        <f t="shared" ref="G37:I37" si="1">F37-SUM(G2:G34)</f>
         <v>180</v>
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>108</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated branch with beta
</commit_message>
<xml_diff>
--- a/Background Documentation/Burndown Chart/Burndown_Chart.xlsx
+++ b/Background Documentation/Burndown Chart/Burndown_Chart.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maddy Carden\Documents\UNI\Semester 1 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maddy Carden\Documents\UNI\Semester 2 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A34D0E-1C75-4C68-8F07-D656E69F4CEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F89C2FFE-0ABD-4645-86BB-EE34303A6ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1C7A58D7-4E6D-4B99-A39A-FCECED6FF1E1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Semester 2" sheetId="2" r:id="rId1"/>
+    <sheet name="Semester 1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>User Story</t>
   </si>
@@ -169,13 +170,64 @@
   </si>
   <si>
     <t>Start</t>
+  </si>
+  <si>
+    <t>1.1.9. As a user, I want to detect and access the ambient light sensor so that I can gather ambient light data</t>
+  </si>
+  <si>
+    <t>1.1.10. As a user, I want to detect and access the GPS so that I can gather latitude and longitude data</t>
+  </si>
+  <si>
+    <t>1.1.11. As a user, I want microphone data to be collected without lag in real time so that all my data can be collected in unison</t>
+  </si>
+  <si>
+    <t>1.2.8. As a user I want to collect illuminance from the ambient light sensor so that I have this data for my experiment</t>
+  </si>
+  <si>
+    <t>1.2.9. As a user I want to collect latitude and longitude from the GPS so that I have this data for my experiment</t>
+  </si>
+  <si>
+    <t>2.2.7. As a user I want to generate and update a graph for ambient light luminosity data in real-time, so that I can view my collected data</t>
+  </si>
+  <si>
+    <t>2.2.8. As a user I want to generate and update a graph for GPS latitude and longitude data in real-time so that I can view my collected data</t>
+  </si>
+  <si>
+    <t>3.1.8. As a user I want to store the collected ambient light luminosity, so that I can use it later</t>
+  </si>
+  <si>
+    <t>3.1.9. As a user I want to store the collected GPS latitude and longitude data, so that I can use it later</t>
+  </si>
+  <si>
+    <t>3.2.4. As a user, I want to delete data that I have exported, so that my device storage doesn't fill up with data once I have finished using it</t>
+  </si>
+  <si>
+    <t>4.1.1. As a developer, I want to obtain ethical clearance so that I can test the application with disabled individuals</t>
+  </si>
+  <si>
+    <t>4.1.2. As a developer, I want to test the application with disabled users so that I can optimize the usability of the application</t>
+  </si>
+  <si>
+    <t>4.1.3. As a product owner, I want an apk, so that I can test the android app myself</t>
+  </si>
+  <si>
+    <t>4.1.4. As a product owner, I want an ipa so that I can test the iOS app myself</t>
+  </si>
+  <si>
+    <t>Sprint 9</t>
+  </si>
+  <si>
+    <t>Sprint 10</t>
+  </si>
+  <si>
+    <t>Ideal work remaining</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +248,19 @@
       <color rgb="FF1A1A1A"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,10 +283,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,6 +306,472 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Sensible Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal work remaining</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Semester 2'!$C$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sprint 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Sprint 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sprint 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sprint 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Sprint 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Semester 2'!$C$19:$M$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>163.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>145.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>127.40000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>109.20000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91.000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72.800000000000011</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F7F0-4C7D-A920-8F630EB03D2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual work remaining</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Semester 2'!$C$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sprint 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Sprint 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sprint 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sprint 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Sprint 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Semester 2'!$C$18:$M$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-F7F0-4C7D-A920-8F630EB03D2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="221237856"/>
+        <c:axId val="221238688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="221237856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="221238688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="221238688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="221237856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -324,7 +856,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$36</c:f>
+              <c:f>'Semester 1'!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -347,7 +879,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:f>'Semester 1'!$B$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -382,7 +914,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$36:$J$36</c:f>
+              <c:f>'Semester 1'!$B$36:$J$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -428,7 +960,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$37</c:f>
+              <c:f>'Semester 1'!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -451,7 +983,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:f>'Semester 1'!$B$1:$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -486,7 +1018,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$37:$J$37</c:f>
+              <c:f>'Semester 1'!$B$37:$J$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -509,7 +1041,10 @@
                   <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>111</c:v>
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -818,6 +1353,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1334,7 +1909,564 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95557</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>26230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>311274</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>149411</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EBF2B69-DDAA-4DC8-A972-C8CAAB024B4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1671,14 +2803,339 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8D38B7-E15B-446D-AF9D-70DAFFF397FD}">
+  <dimension ref="A1:M34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="51" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="52.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <f>SUM(C2:C15)</f>
+        <v>182</v>
+      </c>
+      <c r="D18">
+        <f>C18-SUM(D5:D15)</f>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>182</v>
+      </c>
+      <c r="D19">
+        <f>C19-18.2</f>
+        <v>163.80000000000001</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:M19" si="0">D19-18.2</f>
+        <v>145.60000000000002</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>127.40000000000002</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>109.20000000000002</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>91.000000000000014</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>72.800000000000011</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>54.600000000000009</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>36.400000000000006</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>18.200000000000006</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF4A8D6-7B70-4B05-B2EF-CB4408646652}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="47" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J34"/>
+    <sheetView zoomScale="40" workbookViewId="0">
+      <selection sqref="A1:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1744,6 +3201,12 @@
       <c r="H2">
         <v>6</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1770,6 +3233,12 @@
       <c r="H3">
         <v>0</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -1796,6 +3265,12 @@
       <c r="H4">
         <v>6</v>
       </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -1822,6 +3297,12 @@
       <c r="H5">
         <v>0</v>
       </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -1848,6 +3329,12 @@
       <c r="H6">
         <v>6</v>
       </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
@@ -1874,6 +3361,12 @@
       <c r="H7">
         <v>0</v>
       </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -1900,6 +3393,12 @@
       <c r="H8">
         <v>0</v>
       </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
@@ -1924,6 +3423,12 @@
         <v>0</v>
       </c>
       <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
         <v>0</v>
       </c>
     </row>
@@ -1952,6 +3457,12 @@
       <c r="H10">
         <v>8</v>
       </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
@@ -1978,6 +3489,12 @@
       <c r="H11">
         <v>0</v>
       </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
@@ -2004,6 +3521,12 @@
       <c r="H12">
         <v>8</v>
       </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
@@ -2030,6 +3553,12 @@
       <c r="H13">
         <v>8</v>
       </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
@@ -2056,6 +3585,12 @@
       <c r="H14">
         <v>0</v>
       </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
@@ -2082,6 +3617,12 @@
       <c r="H15">
         <v>0</v>
       </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
@@ -2108,8 +3649,14 @@
       <c r="H16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -2134,8 +3681,14 @@
       <c r="H17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -2160,8 +3713,14 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -2186,8 +3745,14 @@
       <c r="H19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2212,8 +3777,14 @@
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -2238,8 +3809,14 @@
       <c r="H21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2264,8 +3841,14 @@
       <c r="H22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2290,8 +3873,14 @@
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2316,8 +3905,14 @@
       <c r="H24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2342,8 +3937,14 @@
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25">
+        <v>8</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2368,8 +3969,14 @@
       <c r="H26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -2394,8 +4001,14 @@
       <c r="H27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27">
+        <v>8</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2420,8 +4033,14 @@
       <c r="H28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -2446,8 +4065,14 @@
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29">
+        <v>8</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2472,8 +4097,14 @@
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30">
+        <v>8</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -2498,8 +4129,14 @@
       <c r="H31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -2522,6 +4159,12 @@
         <v>0</v>
       </c>
       <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>8</v>
+      </c>
+      <c r="J32">
         <v>0</v>
       </c>
     </row>
@@ -2550,6 +4193,12 @@
       <c r="H33">
         <v>0</v>
       </c>
+      <c r="I33">
+        <v>8</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
@@ -2576,6 +4225,12 @@
       <c r="H34">
         <v>0</v>
       </c>
+      <c r="I34">
+        <v>13</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
@@ -2642,12 +4297,16 @@
         <v>223</v>
       </c>
       <c r="G37">
-        <f t="shared" ref="G37:J37" si="1">F37-SUM(G2:G34)</f>
+        <f t="shared" ref="G37:I37" si="1">F37-SUM(G2:G34)</f>
         <v>180</v>
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>108</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>